<commit_message>
added PCB for BOSH PMP180 revised WE28 schemaitc with added text
</commit_message>
<xml_diff>
--- a/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
+++ b/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="332">
   <si>
     <t>Qty</t>
   </si>
@@ -900,9 +900,6 @@
     <t>538-42878-6264</t>
   </si>
   <si>
-    <t>720-SFH9201-2/3-Z</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
@@ -1093,6 +1090,24 @@
   </si>
   <si>
     <t>538-08-50-0114</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-470-E3</t>
+  </si>
+  <si>
+    <t>720-SFH9206</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-1.0K-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-330-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-120-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-10K-E3</t>
   </si>
 </sst>
 </file>
@@ -1264,27 +1279,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM_Base" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VPower_feed" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MRF24_Module" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_enc" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="HP03S_HIH6130" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_Tree_connect" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM_Base" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VPower_feed" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MRF24_Module" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1578,9 +1593,9 @@
   <dimension ref="A1:V164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="885" topLeftCell="A97" activePane="bottomLeft"/>
+      <pane ySplit="885" topLeftCell="A82" activePane="bottomLeft"/>
       <selection activeCell="O3" sqref="O3"/>
-      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1636,7 +1651,7 @@
         <v>259</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>74</v>
@@ -1645,10 +1660,10 @@
         <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1671,7 +1686,7 @@
         <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K3" s="1">
         <v>0.48</v>
@@ -1704,7 +1719,7 @@
         <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K4" s="1">
         <v>10.8</v>
@@ -1737,7 +1752,7 @@
         <v>86</v>
       </c>
       <c r="G5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K5" s="1">
         <v>3.1</v>
@@ -1770,7 +1785,7 @@
         <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K6" s="1">
         <v>1.81</v>
@@ -1862,7 +1877,7 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -2135,7 +2150,7 @@
         <v>108</v>
       </c>
       <c r="G18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K18" s="1">
         <v>9.5</v>
@@ -2168,7 +2183,7 @@
         <v>164</v>
       </c>
       <c r="G19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -2204,7 +2219,7 @@
         <v>97</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
@@ -2264,7 +2279,7 @@
         <v>99</v>
       </c>
       <c r="G22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K22" s="1">
         <v>4.83</v>
@@ -2297,7 +2312,7 @@
         <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K23" s="1">
         <v>14.3</v>
@@ -2330,7 +2345,7 @@
         <v>123</v>
       </c>
       <c r="G24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2486,7 +2501,7 @@
         <v>75</v>
       </c>
       <c r="G29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K29" s="1">
         <v>6.7</v>
@@ -2538,7 +2553,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -2553,7 +2568,7 @@
         <v>138</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K31" s="1">
         <v>37</v>
@@ -2571,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C32" t="s">
         <v>105</v>
@@ -2610,7 +2625,7 @@
         <v>96</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K33" s="1">
         <v>17</v>
@@ -2628,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
@@ -2640,7 +2655,7 @@
         <v>104</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K34" s="1">
         <v>2.73</v>
@@ -2667,7 +2682,7 @@
         <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>103</v>
@@ -2694,7 +2709,7 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>102</v>
@@ -2721,7 +2736,7 @@
         <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>101</v>
@@ -2739,10 +2754,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>297</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="K38" s="1">
         <v>20</v>
@@ -2895,7 +2910,7 @@
         <v>82</v>
       </c>
       <c r="G45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K45" s="1">
         <v>2.95</v>
@@ -2955,7 +2970,7 @@
         <v>100</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J47" s="19">
         <v>18</v>
@@ -2973,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C48" t="s">
         <v>118</v>
@@ -2982,7 +2997,7 @@
         <v>118</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K48" s="1">
         <v>16</v>
@@ -3074,7 +3089,7 @@
         <v>99</v>
       </c>
       <c r="G54" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K54" s="1">
         <v>4.83</v>
@@ -3104,7 +3119,7 @@
         <v>75</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K55" s="1">
         <v>6.67</v>
@@ -3119,10 +3134,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>302</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="K56" s="1">
         <v>16</v>
@@ -3204,13 +3219,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C61" t="s">
         <v>213</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K61" s="1">
         <v>16</v>
@@ -3374,7 +3389,7 @@
     </row>
     <row r="72" spans="1:15">
       <c r="A72" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:15">
@@ -3397,10 +3412,10 @@
         <v>255</v>
       </c>
       <c r="G73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J73" s="19">
         <v>2.89</v>
@@ -3460,7 +3475,7 @@
         <v>118</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K75" s="1">
         <v>10.8</v>
@@ -3478,7 +3493,7 @@
         <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -3505,7 +3520,7 @@
         <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
@@ -3529,10 +3544,10 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
+        <v>313</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="K78" s="1">
         <v>5</v>
@@ -3577,10 +3592,10 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K80" s="1">
         <v>16.600000000000001</v>
@@ -3755,7 +3770,7 @@
     </row>
     <row r="92" spans="1:15">
       <c r="A92" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="13.5" customHeight="1">
@@ -3775,7 +3790,7 @@
         <v>179</v>
       </c>
       <c r="G93" t="s">
-        <v>262</v>
+        <v>327</v>
       </c>
       <c r="H93" s="18"/>
       <c r="K93" s="1">
@@ -3832,6 +3847,9 @@
       <c r="F95" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="G95" s="2" t="s">
+        <v>330</v>
+      </c>
       <c r="K95" s="1">
         <v>0.1</v>
       </c>
@@ -3862,6 +3880,9 @@
       <c r="F96" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="G96" s="2" t="s">
+        <v>331</v>
+      </c>
       <c r="K96" s="1">
         <v>0.14000000000000001</v>
       </c>
@@ -3889,6 +3910,9 @@
       <c r="E97" t="s">
         <v>26</v>
       </c>
+      <c r="G97" s="2" t="s">
+        <v>329</v>
+      </c>
       <c r="K97" s="1">
         <v>0.1</v>
       </c>
@@ -3916,6 +3940,9 @@
       <c r="F98" s="2" t="s">
         <v>222</v>
       </c>
+      <c r="G98" t="s">
+        <v>328</v>
+      </c>
       <c r="K98" s="1">
         <v>0.14000000000000001</v>
       </c>
@@ -3935,7 +3962,7 @@
         <v>115</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K99" s="1">
         <v>16.600000000000001</v>
@@ -3981,7 +4008,7 @@
     </row>
     <row r="102" spans="1:22">
       <c r="A102" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B102" s="8"/>
     </row>
@@ -4018,6 +4045,9 @@
       <c r="F104" s="2" t="s">
         <v>162</v>
       </c>
+      <c r="G104" t="s">
+        <v>326</v>
+      </c>
       <c r="K104" s="1">
         <v>0.1</v>
       </c>
@@ -4048,6 +4078,9 @@
       <c r="F105" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="G105" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="K105" s="1">
         <v>0.48</v>
       </c>
@@ -4106,7 +4139,7 @@
         <v>118</v>
       </c>
       <c r="G107" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K107" s="1">
         <v>149.1</v>
@@ -4142,7 +4175,7 @@
         <v>202</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J108" s="19">
         <v>2.5</v>
@@ -4160,10 +4193,10 @@
         <v>1</v>
       </c>
       <c r="B109" t="s">
+        <v>291</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="F109" t="s">
         <v>118</v>
@@ -4190,7 +4223,7 @@
         <v>115</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K110" s="1">
         <v>16.600000000000001</v>
@@ -4222,7 +4255,7 @@
     </row>
     <row r="112" spans="1:22" s="1" customFormat="1">
       <c r="A112" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112"/>
@@ -4279,7 +4312,9 @@
       <c r="F114" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G114" s="2"/>
+      <c r="G114" t="s">
+        <v>326</v>
+      </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="19"/>
@@ -4315,6 +4350,9 @@
       <c r="F115" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="G115" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="K115" s="1">
         <v>0.48</v>
       </c>
@@ -4346,7 +4384,7 @@
         <v>86</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -4381,7 +4419,7 @@
         <v>202</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J117" s="19">
         <v>2.5</v>
@@ -4399,16 +4437,16 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
+        <v>283</v>
+      </c>
+      <c r="C118" t="s">
         <v>284</v>
-      </c>
-      <c r="C118" t="s">
-        <v>285</v>
       </c>
       <c r="D118"/>
       <c r="E118"/>
       <c r="F118"/>
       <c r="G118" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H118"/>
       <c r="I118"/>
@@ -4429,10 +4467,10 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
+        <v>291</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="F119" t="s">
         <v>118</v>
@@ -4463,7 +4501,7 @@
       <c r="E120"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -4691,7 +4729,7 @@
         <v>132</v>
       </c>
       <c r="G128" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H128"/>
       <c r="I128"/>
@@ -4788,7 +4826,7 @@
     </row>
     <row r="133" spans="1:15">
       <c r="A133" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G133" t="s">
         <v>118</v>
@@ -4806,10 +4844,10 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G134" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K134" s="1">
         <v>2.4</v>
@@ -4828,7 +4866,7 @@
         <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C135"/>
       <c r="D135"/>
@@ -5108,54 +5146,54 @@
     </row>
     <row r="162" spans="1:14">
       <c r="A162" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B162" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C162" s="1">
         <f>O39+O49+O121+O136</f>
         <v>60.540780000000005</v>
       </c>
       <c r="D162" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H162" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N162" s="7"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B163" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C163" s="1">
         <f>O101</f>
         <v>7.2670300000000001</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" t="s">
+        <v>318</v>
+      </c>
+      <c r="B164" t="s">
         <v>319</v>
-      </c>
-      <c r="B164" t="s">
-        <v>320</v>
       </c>
       <c r="C164" s="1">
         <f>O81</f>
         <v>9.8590499999999999</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM with Mouser PN's -- Updated Wind-direction DOC and PDF Updated wind dir doc to better reflect the specifications of the new sensor
</commit_message>
<xml_diff>
--- a/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
+++ b/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="339">
   <si>
     <t>Qty</t>
   </si>
@@ -1108,6 +1108,27 @@
   </si>
   <si>
     <t>71-CRCW0603-10K-E3</t>
+  </si>
+  <si>
+    <t>538-42410-8314</t>
+  </si>
+  <si>
+    <t>667-ERJ-3EKF1002V</t>
+  </si>
+  <si>
+    <t>667-ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t>77-VJ0603A220JXACBC</t>
+  </si>
+  <si>
+    <t>859-LTST-C190KFKT</t>
+  </si>
+  <si>
+    <t>859-LTST-C190KRKT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859-LTST-C190KGKT </t>
   </si>
 </sst>
 </file>
@@ -1279,27 +1300,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_Tree_connect" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM_Base" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VPower_feed" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MRF24_Module" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_enc" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="HP03S_HIH6130" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_Tree_connect" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1593,9 +1614,9 @@
   <dimension ref="A1:V164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="885" topLeftCell="A82" activePane="bottomLeft"/>
+      <pane ySplit="885" topLeftCell="A22" activePane="bottomLeft"/>
       <selection activeCell="O3" sqref="O3"/>
-      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1817,6 +1838,9 @@
       <c r="F7" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="G7" s="10" t="s">
+        <v>335</v>
+      </c>
       <c r="K7" s="1">
         <v>0.3</v>
       </c>
@@ -1912,6 +1936,9 @@
       <c r="F10" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>334</v>
+      </c>
       <c r="K10" s="1">
         <v>0.1</v>
       </c>
@@ -1941,6 +1968,9 @@
       </c>
       <c r="F11" s="2" t="s">
         <v>90</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>333</v>
       </c>
       <c r="K11" s="1">
         <v>0.14000000000000001</v>
@@ -2687,6 +2717,9 @@
       <c r="F35" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="G35" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="K35" s="1">
         <v>0.78</v>
       </c>
@@ -2714,6 +2747,9 @@
       <c r="F36" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="G36" s="2" t="s">
+        <v>338</v>
+      </c>
       <c r="K36" s="1">
         <v>0.74</v>
       </c>
@@ -2740,6 +2776,9 @@
       </c>
       <c r="F37" s="2" t="s">
         <v>101</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="K37" s="1">
         <v>0.78</v>
@@ -3205,6 +3244,9 @@
       </c>
       <c r="F60" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="G60" t="s">
+        <v>332</v>
       </c>
       <c r="K60" s="1">
         <v>7.47</v>
@@ -5200,9 +5242,10 @@
   <hyperlinks>
     <hyperlink ref="E64" r:id="rId1"/>
     <hyperlink ref="E84" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3" tooltip="Click to view additional information on this product." display="http://www.mouser.com/ProductDetail/Vishay-Vitramon/VJ0603A220JXACW1BC/?qs=sGAEpiMZZMs0AnBnWHyRQMqfda103KBdBdiLJaMBFC0%3d"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="30" fitToHeight="2" orientation="portrait" r:id="rId3"/>
+  <pageSetup scale="30" fitToHeight="2" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed BOM to reflect new MRF24WG module
</commit_message>
<xml_diff>
--- a/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
+++ b/Hardware/Wifi_WX_Station/BOMStuff/BOM_STATION_all.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="340">
   <si>
     <t>Qty</t>
   </si>
@@ -294,12 +294,6 @@
     <t>2X5-RA-HEADER</t>
   </si>
   <si>
-    <t>MRF24WB0MA</t>
-  </si>
-  <si>
-    <t>MRF24W</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -414,9 +408,6 @@
     <t>ED2992CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve"> MRF24WB0MB/RM-ND</t>
-  </si>
-  <si>
     <t>475-2512-1-ND</t>
   </si>
   <si>
@@ -909,9 +900,6 @@
     <t>Future</t>
   </si>
   <si>
-    <t>EZ-Shopfun</t>
-  </si>
-  <si>
     <t>511-LD29150DT33R</t>
   </si>
   <si>
@@ -1129,6 +1117,21 @@
   </si>
   <si>
     <t xml:space="preserve">859-LTST-C190KGKT </t>
+  </si>
+  <si>
+    <t>MRF24WG0MA</t>
+  </si>
+  <si>
+    <t>MRF24WG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MRF24WG0MB/RM-ND</t>
+  </si>
+  <si>
+    <t>e-bay</t>
+  </si>
+  <si>
+    <t>digitalrepair@hotmail.com&lt;digitalrepair@hotmail.com&gt;;</t>
   </si>
 </sst>
 </file>
@@ -1300,27 +1303,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_enc" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="HP03S_HIH6130" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_Tree_connect" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="BOM_Base" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VPower_feed" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MRF24_Module" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wind_enc" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="HP03S_HIH6130" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1616,7 +1619,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="885" topLeftCell="A22" activePane="bottomLeft"/>
       <selection activeCell="O3" sqref="O3"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1639,7 +1642,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -1660,31 +1663,31 @@
         <v>3</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="O2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1692,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1701,13 +1704,13 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K3" s="1">
         <v>0.48</v>
@@ -1725,22 +1728,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K4" s="1">
         <v>10.8</v>
@@ -1758,22 +1761,22 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="G5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K5" s="1">
         <v>3.1</v>
@@ -1791,7 +1794,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -1803,10 +1806,10 @@
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="K6" s="1">
         <v>1.81</v>
@@ -1824,7 +1827,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1836,10 +1839,10 @@
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="K7" s="1">
         <v>0.3</v>
@@ -1854,19 +1857,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
@@ -1888,20 +1891,20 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -1922,22 +1925,22 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="K10" s="1">
         <v>0.1</v>
@@ -1955,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
@@ -1964,13 +1967,13 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="K11" s="1">
         <v>0.14000000000000001</v>
@@ -1988,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1997,10 +2000,10 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K12" s="1">
         <v>0.1</v>
@@ -2018,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -2030,7 +2033,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K13" s="1">
         <v>0.1</v>
@@ -2048,7 +2051,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
         <v>55</v>
@@ -2057,10 +2060,10 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K14" s="1">
         <v>0.1</v>
@@ -2078,19 +2081,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K15" s="1">
         <v>0.1</v>
@@ -2108,19 +2111,19 @@
         <v>1</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K16" s="1">
         <v>0.1</v>
@@ -2135,19 +2138,19 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K17" s="1">
         <v>0.14000000000000001</v>
@@ -2165,10 +2168,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -2177,10 +2180,10 @@
         <v>21</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="K18" s="1">
         <v>9.5</v>
@@ -2204,16 +2207,16 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G19" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -2246,10 +2249,10 @@
         <v>29</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="K20" s="1">
         <v>1</v>
@@ -2267,19 +2270,19 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" t="s">
+        <v>215</v>
+      </c>
+      <c r="E21" t="s">
         <v>216</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="D21" t="s">
-        <v>218</v>
-      </c>
-      <c r="E21" t="s">
-        <v>219</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="K21" s="1">
         <v>3</v>
@@ -2306,10 +2309,10 @@
         <v>37</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G22" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K22" s="1">
         <v>4.83</v>
@@ -2327,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
@@ -2339,10 +2342,10 @@
         <v>33</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="K23" s="1">
         <v>14.3</v>
@@ -2360,22 +2363,22 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G24" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
@@ -2396,19 +2399,19 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D25" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" t="s">
         <v>167</v>
-      </c>
-      <c r="F25" t="s">
-        <v>170</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
@@ -2427,19 +2430,19 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D26" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E26" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K26" s="1">
         <v>3.05</v>
@@ -2454,19 +2457,19 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D27" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E27" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
@@ -2485,19 +2488,19 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
       <c r="F28" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -2516,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C29" t="s">
         <v>42</v>
@@ -2528,10 +2531,10 @@
         <v>44</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K29" s="1">
         <v>6.7</v>
@@ -2549,20 +2552,20 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
@@ -2583,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
@@ -2595,10 +2598,10 @@
         <v>41</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="K31" s="1">
         <v>37</v>
@@ -2616,16 +2619,16 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K32" s="1">
         <v>51.8</v>
@@ -2640,22 +2643,22 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K33" s="1">
         <v>17</v>
@@ -2673,19 +2676,19 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K34" s="1">
         <v>2.73</v>
@@ -2712,13 +2715,13 @@
         <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="K35" s="1">
         <v>0.78</v>
@@ -2742,13 +2745,13 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="K36" s="1">
         <v>0.74</v>
@@ -2772,13 +2775,13 @@
         <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="K37" s="1">
         <v>0.78</v>
@@ -2793,10 +2796,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="K38" s="1">
         <v>20</v>
@@ -2818,7 +2821,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B40" s="8"/>
     </row>
@@ -2844,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -2856,7 +2859,7 @@
         <v>52</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K42" s="1">
         <v>0.48</v>
@@ -2874,7 +2877,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
         <v>53</v>
@@ -2886,7 +2889,7 @@
         <v>54</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K43" s="1">
         <v>0.1</v>
@@ -2904,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
         <v>55</v>
@@ -2916,7 +2919,7 @@
         <v>56</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K44" s="1">
         <v>0.1</v>
@@ -2934,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
         <v>57</v>
@@ -2946,10 +2949,10 @@
         <v>25</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G45" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="K45" s="1">
         <v>2.95</v>
@@ -2967,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
         <v>58</v>
@@ -2979,7 +2982,7 @@
         <v>5</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K46" s="1">
         <v>3.56</v>
@@ -2994,25 +2997,28 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C47" t="s">
+        <v>335</v>
+      </c>
+      <c r="D47" t="s">
+        <v>336</v>
+      </c>
+      <c r="E47" t="s">
         <v>60</v>
       </c>
-      <c r="D47" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" t="s">
-        <v>62</v>
-      </c>
       <c r="F47" s="2" t="s">
-        <v>100</v>
+        <v>337</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>265</v>
+        <v>338</v>
       </c>
       <c r="J47" s="19">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="K47" s="1">
         <v>210</v>
@@ -3027,16 +3033,16 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C48" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K48" s="1">
         <v>16</v>
@@ -3058,7 +3064,7 @@
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B51" s="8"/>
       <c r="N51" s="21"/>
@@ -3085,16 +3091,16 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E53" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F53" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G53"/>
       <c r="H53"/>
@@ -3125,10 +3131,10 @@
         <v>37</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G54" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K54" s="1">
         <v>4.83</v>
@@ -3152,13 +3158,13 @@
         <v>43</v>
       </c>
       <c r="E55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K55" s="1">
         <v>6.67</v>
@@ -3173,10 +3179,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K56" s="1">
         <v>16</v>
@@ -3198,7 +3204,7 @@
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F58"/>
       <c r="G58"/>
@@ -3243,10 +3249,10 @@
         <v>44</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G60" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="K60" s="1">
         <v>7.47</v>
@@ -3261,13 +3267,13 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K61" s="1">
         <v>16</v>
@@ -3289,7 +3295,7 @@
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B63" s="8"/>
     </row>
@@ -3298,14 +3304,14 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D64"/>
       <c r="E64" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -3326,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F65"/>
       <c r="G65"/>
@@ -3346,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K66" s="1">
         <v>25</v>
@@ -3361,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K67" s="1">
         <v>40</v>
@@ -3376,7 +3382,7 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K68" s="1">
         <v>10</v>
@@ -3391,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K69" s="24">
         <v>50</v>
@@ -3406,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K70" s="1">
         <v>75</v>
@@ -3431,7 +3437,7 @@
     </row>
     <row r="72" spans="1:15">
       <c r="A72" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:15">
@@ -3439,25 +3445,25 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D73" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E73" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G73" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J73" s="19">
         <v>2.89</v>
@@ -3475,19 +3481,19 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
       </c>
       <c r="D74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E74" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K74" s="1">
         <v>3.05</v>
@@ -3502,22 +3508,22 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C75" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D75" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E75" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K75" s="1">
         <v>10.8</v>
@@ -3532,19 +3538,19 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C76" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K76" s="1">
         <v>0.1</v>
@@ -3559,10 +3565,10 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C77" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
@@ -3571,7 +3577,7 @@
         <v>54</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K77" s="1">
         <v>0.1</v>
@@ -3586,10 +3592,10 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K78" s="1">
         <v>5</v>
@@ -3604,10 +3610,10 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C79" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D79" t="s">
         <v>8</v>
@@ -3616,7 +3622,7 @@
         <v>56</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K79" s="1">
         <v>0.1</v>
@@ -3634,10 +3640,10 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K80" s="1">
         <v>16.600000000000001</v>
@@ -3649,29 +3655,29 @@
     </row>
     <row r="81" spans="1:15" ht="14.25" customHeight="1">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G81"/>
       <c r="H81"/>
       <c r="I81"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N81" s="23">
         <f>SUM(N73:N80)</f>
@@ -3687,7 +3693,7 @@
     </row>
     <row r="83" spans="1:15">
       <c r="A83" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:15" s="1" customFormat="1">
@@ -3695,14 +3701,14 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C84" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D84"/>
       <c r="E84" s="10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3723,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K85" s="1">
         <v>60</v>
@@ -3741,7 +3747,7 @@
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K86" s="1">
         <v>25</v>
@@ -3756,7 +3762,7 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K87" s="1">
         <v>40</v>
@@ -3771,7 +3777,7 @@
         <v>2</v>
       </c>
       <c r="B88" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K88" s="1">
         <v>10</v>
@@ -3786,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="K89" s="24">
         <v>50</v>
@@ -3812,7 +3818,7 @@
     </row>
     <row r="92" spans="1:15">
       <c r="A92" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="13.5" customHeight="1">
@@ -3820,19 +3826,19 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C93" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E93" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G93" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H93" s="18"/>
       <c r="K93" s="1">
@@ -3851,16 +3857,16 @@
         <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C94" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E94" t="s">
+        <v>177</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="K94" s="1">
         <v>2.0699999999999998</v>
@@ -3875,22 +3881,22 @@
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C95" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
       </c>
       <c r="E95" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="K95" s="1">
         <v>0.1</v>
@@ -3908,7 +3914,7 @@
         <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C96" t="s">
         <v>53</v>
@@ -3917,13 +3923,13 @@
         <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K96" s="1">
         <v>0.14000000000000001</v>
@@ -3941,10 +3947,10 @@
         <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D97" t="s">
         <v>8</v>
@@ -3953,7 +3959,7 @@
         <v>26</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="K97" s="1">
         <v>0.1</v>
@@ -3968,22 +3974,22 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
       </c>
       <c r="E98" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G98" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K98" s="1">
         <v>0.14000000000000001</v>
@@ -4001,10 +4007,10 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K99" s="1">
         <v>16.600000000000001</v>
@@ -4022,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K100" s="1">
         <v>40</v>
@@ -4034,10 +4040,10 @@
     </row>
     <row r="101" spans="1:22">
       <c r="K101" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N101" s="23">
         <f>SUM(N93:N100)</f>
@@ -4050,7 +4056,7 @@
     </row>
     <row r="102" spans="1:22">
       <c r="A102" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B102" s="8"/>
     </row>
@@ -4073,22 +4079,22 @@
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C104" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D104" t="s">
         <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G104" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="K104" s="1">
         <v>0.1</v>
@@ -4106,7 +4112,7 @@
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
@@ -4115,13 +4121,13 @@
         <v>7</v>
       </c>
       <c r="E105" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K105" s="1">
         <v>0.48</v>
@@ -4139,19 +4145,19 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D106" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E106" t="s">
         <v>25</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K106" s="1">
         <v>4.6900000000000004</v>
@@ -4166,22 +4172,22 @@
         <v>1</v>
       </c>
       <c r="B107" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D107" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E107" t="s">
         <v>33</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G107" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="K107" s="1">
         <v>149.1</v>
@@ -4191,10 +4197,10 @@
         <v>14.91</v>
       </c>
       <c r="S107" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="V107" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:22">
@@ -4202,22 +4208,22 @@
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D108" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E108" t="s">
         <v>19</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J108" s="19">
         <v>2.5</v>
@@ -4235,16 +4241,16 @@
         <v>1</v>
       </c>
       <c r="B109" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F109" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G109" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H109"/>
       <c r="I109"/>
@@ -4262,10 +4268,10 @@
         <v>1</v>
       </c>
       <c r="B110" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="K110" s="1">
         <v>16.600000000000001</v>
@@ -4297,7 +4303,7 @@
     </row>
     <row r="112" spans="1:22" s="1" customFormat="1">
       <c r="A112" s="9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112"/>
@@ -4340,22 +4346,22 @@
         <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D114" t="s">
         <v>8</v>
       </c>
       <c r="E114" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G114" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -4378,7 +4384,7 @@
         <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
@@ -4387,13 +4393,13 @@
         <v>7</v>
       </c>
       <c r="E115" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K115" s="1">
         <v>0.48</v>
@@ -4411,22 +4417,22 @@
         <v>1</v>
       </c>
       <c r="B116" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D116" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E116" t="s">
         <v>25</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -4446,22 +4452,22 @@
         <v>1</v>
       </c>
       <c r="B117" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D117" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E117" t="s">
         <v>19</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J117" s="19">
         <v>2.5</v>
@@ -4479,16 +4485,16 @@
         <v>1</v>
       </c>
       <c r="B118" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C118" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D118"/>
       <c r="E118"/>
       <c r="F118"/>
       <c r="G118" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H118"/>
       <c r="I118"/>
@@ -4509,16 +4515,16 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F119" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G119" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H119"/>
       <c r="I119"/>
@@ -4536,14 +4542,14 @@
         <v>1</v>
       </c>
       <c r="B120" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C120"/>
       <c r="D120"/>
       <c r="E120"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -4580,7 +4586,7 @@
     </row>
     <row r="122" spans="1:15" s="1" customFormat="1">
       <c r="A122" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B122"/>
       <c r="C122"/>
@@ -4598,17 +4604,17 @@
         <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C123" t="s">
+        <v>182</v>
+      </c>
+      <c r="D123" t="s">
         <v>185</v>
-      </c>
-      <c r="D123" t="s">
-        <v>188</v>
       </c>
       <c r="E123"/>
       <c r="F123" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G123"/>
       <c r="H123"/>
@@ -4630,17 +4636,17 @@
         <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C124" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D124" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E124"/>
       <c r="F124" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G124"/>
       <c r="H124"/>
@@ -4662,7 +4668,7 @@
         <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -4674,7 +4680,7 @@
         <v>52</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
@@ -4698,17 +4704,17 @@
         <v>1</v>
       </c>
       <c r="B126" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C126" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D126"/>
       <c r="E126" t="s">
         <v>56</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
@@ -4731,15 +4737,15 @@
         <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C127" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D127"/>
       <c r="E127"/>
       <c r="F127" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G127"/>
       <c r="H127"/>
@@ -4762,16 +4768,16 @@
         <v>3</v>
       </c>
       <c r="B128" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C128"/>
       <c r="D128"/>
       <c r="E128"/>
       <c r="F128" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G128" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="H128"/>
       <c r="I128"/>
@@ -4793,10 +4799,10 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C129" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D129"/>
       <c r="E129"/>
@@ -4809,7 +4815,7 @@
         <v>10</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M129"/>
       <c r="N129" s="6">
@@ -4868,16 +4874,16 @@
     </row>
     <row r="133" spans="1:15">
       <c r="A133" s="16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="G133" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="O133" s="1"/>
     </row>
@@ -4886,10 +4892,10 @@
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G134" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="K134" s="1">
         <v>2.4</v>
@@ -4908,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C135"/>
       <c r="D135"/>
@@ -4958,10 +4964,10 @@
     </row>
     <row r="148" spans="1:15">
       <c r="A148" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="149" spans="1:15">
@@ -4969,13 +4975,13 @@
         <v>1</v>
       </c>
       <c r="B149" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C149" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K149" s="1">
         <v>100</v>
@@ -4990,13 +4996,13 @@
         <v>1</v>
       </c>
       <c r="B150" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C150" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K150" s="1">
         <v>70</v>
@@ -5011,13 +5017,13 @@
         <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C151" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K151" s="1">
         <v>50</v>
@@ -5032,13 +5038,13 @@
         <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C152" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K152" s="1">
         <v>24.64</v>
@@ -5053,10 +5059,10 @@
         <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F153" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G153"/>
       <c r="H153"/>
@@ -5075,13 +5081,13 @@
         <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C154" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F154" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G154"/>
       <c r="H154"/>
@@ -5100,7 +5106,7 @@
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F155"/>
       <c r="G155"/>
@@ -5120,7 +5126,7 @@
         <v>1</v>
       </c>
       <c r="B156" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K156" s="1">
         <v>50</v>
@@ -5135,11 +5141,11 @@
         <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E157" s="10"/>
       <c r="F157" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K157" s="1">
         <v>120</v>
@@ -5155,10 +5161,10 @@
         <v>1</v>
       </c>
       <c r="B158" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K158" s="1">
         <v>50</v>
@@ -5188,54 +5194,54 @@
     </row>
     <row r="162" spans="1:14">
       <c r="A162" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B162" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C162" s="1">
         <f>O39+O49+O121+O136</f>
         <v>60.540780000000005</v>
       </c>
       <c r="D162" t="s">
+        <v>312</v>
+      </c>
+      <c r="F162" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F162" s="2" t="s">
-        <v>320</v>
-      </c>
       <c r="H162" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="N162" s="7"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B163" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C163" s="1">
         <f>O101</f>
         <v>7.2670300000000001</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="164" spans="1:14">
       <c r="A164" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B164" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C164" s="1">
         <f>O81</f>
         <v>9.8590499999999999</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>